<commit_message>
Revert "Merge branch 'main' of https://github.com/ssf-czh/analy_pro"
This reverts commit cc3b51effa5fe8fc7d2992b6474c621c56036638, reversing
changes made to eb9561ba72a56137dea7b7a2214f2765c27a19bb.
</commit_message>
<xml_diff>
--- a/model/template.xlsx
+++ b/model/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="10380" activeTab="5"/>
+    <workbookView windowWidth="24225" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="参数初始值设定" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="128">
   <si>
     <r>
       <rPr>
@@ -390,18 +390,6 @@
     <t>E3</t>
   </si>
   <si>
-    <t>年</t>
-  </si>
-  <si>
-    <t>月</t>
-  </si>
-  <si>
-    <t>日</t>
-  </si>
-  <si>
-    <t>时</t>
-  </si>
-  <si>
     <t>负荷Q/Kw</t>
   </si>
   <si>
@@ -480,6 +468,18 @@
     <t>设备开启台数/台</t>
   </si>
   <si>
+    <t>年</t>
+  </si>
+  <si>
+    <t>月</t>
+  </si>
+  <si>
+    <t>日</t>
+  </si>
+  <si>
+    <t>时</t>
+  </si>
+  <si>
     <t>负荷Q，Kw</t>
   </si>
   <si>
@@ -524,19 +524,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="0.0_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0.000_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.000_ "/>
+    <numFmt numFmtId="178" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -573,7 +573,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -581,14 +581,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -634,10 +634,138 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -645,135 +773,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -809,7 +809,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -821,13 +833,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,7 +893,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,7 +911,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,37 +935,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,31 +947,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -947,31 +965,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -983,13 +989,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1005,71 +1005,56 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1078,7 +1063,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1099,6 +1093,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1113,17 +1122,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1139,20 +1142,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1161,148 +1161,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="29" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1310,150 +1310,150 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1582,7 +1582,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1606,9 +1606,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1632,7 +1632,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1685,7 +1685,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1710,7 +1710,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1724,16 +1724,16 @@
   <sheetPr/>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="31.6428571428571" customWidth="true"/>
+    <col min="1" max="1" width="31.6416666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="37.75" spans="1:10">
+    <row r="1" ht="38.25" spans="1:10">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="19.25" spans="1:10">
+    <row r="2" ht="19.5" spans="1:10">
       <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="16.75" spans="1:10">
+    <row r="3" ht="15" spans="1:10">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -1811,7 +1811,7 @@
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" ht="16.75" spans="1:10">
+    <row r="4" ht="15" spans="1:10">
       <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
@@ -1827,7 +1827,7 @@
       <c r="I4" s="30"/>
       <c r="J4" s="30"/>
     </row>
-    <row r="5" ht="16.75" spans="1:10">
+    <row r="5" ht="15" spans="1:10">
       <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
@@ -1843,7 +1843,7 @@
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
     </row>
-    <row r="6" ht="16.75" spans="1:10">
+    <row r="6" ht="15" spans="1:10">
       <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
     </row>
-    <row r="7" ht="16.75" spans="1:10">
+    <row r="7" ht="15" spans="1:10">
       <c r="A7" s="30" t="s">
         <v>7</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="I7" s="30"/>
       <c r="J7" s="30"/>
     </row>
-    <row r="8" ht="16.75" spans="1:10">
+    <row r="8" ht="15" spans="1:10">
       <c r="A8" s="29" t="s">
         <v>8</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="I8" s="30"/>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" ht="16.75" spans="1:10">
+    <row r="9" ht="15" spans="1:10">
       <c r="A9" s="30" t="s">
         <v>9</v>
       </c>
@@ -1907,7 +1907,7 @@
       <c r="I9" s="30"/>
       <c r="J9" s="30"/>
     </row>
-    <row r="10" ht="16.75" spans="1:10">
+    <row r="10" ht="15" spans="1:10">
       <c r="A10" s="30" t="s">
         <v>10</v>
       </c>
@@ -1923,7 +1923,7 @@
       <c r="I10" s="30"/>
       <c r="J10" s="30"/>
     </row>
-    <row r="11" ht="16.75" spans="1:10">
+    <row r="11" ht="15" spans="1:10">
       <c r="A11" s="30" t="s">
         <v>11</v>
       </c>
@@ -1939,7 +1939,7 @@
       <c r="I11" s="30"/>
       <c r="J11" s="30"/>
     </row>
-    <row r="12" ht="16.75" spans="1:10">
+    <row r="12" ht="15" spans="1:10">
       <c r="A12" s="30" t="s">
         <v>12</v>
       </c>
@@ -1955,7 +1955,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="30"/>
     </row>
-    <row r="13" ht="16.75" spans="1:10">
+    <row r="13" ht="15" spans="1:10">
       <c r="A13" s="29" t="s">
         <v>13</v>
       </c>
@@ -1969,7 +1969,7 @@
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
     </row>
-    <row r="14" ht="16.75" spans="1:10">
+    <row r="14" ht="15" spans="1:10">
       <c r="A14" s="30" t="s">
         <v>14</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="I14" s="30"/>
       <c r="J14" s="30"/>
     </row>
-    <row r="15" ht="16.75" spans="1:10">
+    <row r="15" ht="15" spans="1:10">
       <c r="A15" s="30" t="s">
         <v>15</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
     </row>
-    <row r="16" ht="16.75" spans="1:10">
+    <row r="16" ht="15" spans="1:10">
       <c r="A16" s="30" t="s">
         <v>16</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="I16" s="30"/>
       <c r="J16" s="30"/>
     </row>
-    <row r="17" ht="16.75" spans="1:10">
+    <row r="17" ht="15" spans="1:10">
       <c r="A17" s="30" t="s">
         <v>17</v>
       </c>
@@ -2033,7 +2033,7 @@
       <c r="I17" s="30"/>
       <c r="J17" s="30"/>
     </row>
-    <row r="18" ht="16.75" spans="1:10">
+    <row r="18" ht="15" spans="1:10">
       <c r="A18" s="29" t="s">
         <v>18</v>
       </c>
@@ -2047,7 +2047,7 @@
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
     </row>
-    <row r="19" ht="16.75" spans="1:10">
+    <row r="19" ht="15" spans="1:10">
       <c r="A19" s="30" t="s">
         <v>19</v>
       </c>
@@ -2063,7 +2063,7 @@
       <c r="I19" s="30"/>
       <c r="J19" s="30"/>
     </row>
-    <row r="20" ht="16.75" spans="1:10">
+    <row r="20" ht="15" spans="1:10">
       <c r="A20" s="30" t="s">
         <v>20</v>
       </c>
@@ -2079,7 +2079,7 @@
       <c r="I20" s="30"/>
       <c r="J20" s="30"/>
     </row>
-    <row r="21" ht="16.75" spans="1:10">
+    <row r="21" ht="15" spans="1:10">
       <c r="A21" s="30" t="s">
         <v>21</v>
       </c>
@@ -2095,7 +2095,7 @@
       <c r="I21" s="30"/>
       <c r="J21" s="30"/>
     </row>
-    <row r="22" ht="16.75" spans="1:10">
+    <row r="22" ht="15" spans="1:10">
       <c r="A22" s="30" t="s">
         <v>22</v>
       </c>
@@ -2111,7 +2111,7 @@
       <c r="I22" s="30"/>
       <c r="J22" s="30"/>
     </row>
-    <row r="23" ht="16.75" spans="1:10">
+    <row r="23" ht="15" spans="1:10">
       <c r="A23" s="29" t="s">
         <v>23</v>
       </c>
@@ -2125,7 +2125,7 @@
       <c r="I23" s="30"/>
       <c r="J23" s="30"/>
     </row>
-    <row r="24" ht="19.25" spans="1:10">
+    <row r="24" ht="19.5" spans="1:10">
       <c r="A24" s="31" t="s">
         <v>24</v>
       </c>
@@ -2143,7 +2143,7 @@
       <c r="I24" s="30"/>
       <c r="J24" s="30"/>
     </row>
-    <row r="25" ht="19.25" spans="1:10">
+    <row r="25" ht="19.5" spans="1:10">
       <c r="A25" s="31" t="s">
         <v>25</v>
       </c>
@@ -2161,7 +2161,7 @@
       <c r="I25" s="30"/>
       <c r="J25" s="30"/>
     </row>
-    <row r="26" ht="19.25" spans="1:10">
+    <row r="26" ht="19.5" spans="1:10">
       <c r="A26" s="31" t="s">
         <v>26</v>
       </c>
@@ -2177,7 +2177,7 @@
       <c r="I26" s="31"/>
       <c r="J26" s="31"/>
     </row>
-    <row r="27" ht="19.25" spans="1:10">
+    <row r="27" ht="19.5" spans="1:10">
       <c r="A27" s="31" t="s">
         <v>27</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
     </row>
-    <row r="28" ht="19.25" spans="1:10">
+    <row r="28" ht="19.5" spans="1:10">
       <c r="A28" s="31" t="s">
         <v>28</v>
       </c>
@@ -2209,7 +2209,7 @@
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
     </row>
-    <row r="29" ht="19.25" spans="1:10">
+    <row r="29" ht="19.5" spans="1:10">
       <c r="A29" s="31" t="s">
         <v>29</v>
       </c>
@@ -2240,9 +2240,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
   <sheetData>
-    <row r="1" ht="32" spans="1:8">
+    <row r="1" ht="34.5" spans="1:8">
       <c r="A1" s="19" t="s">
         <v>30</v>
       </c>
@@ -2264,11 +2264,11 @@
       <c r="G1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" ht="16" spans="1:8">
+    <row r="2" ht="17.25" spans="1:8">
       <c r="A2" s="19" t="s">
         <v>38</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="C2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="21" t="s">
@@ -2290,28 +2290,28 @@
       <c r="G2" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="23">
+      <c r="A3" s="24">
         <v>100</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="24">
         <v>2813</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="24">
         <v>541</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="24">
         <v>6</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>10</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="24">
         <v>34</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="24">
         <v>38</v>
       </c>
       <c r="H3" s="25">
@@ -2319,25 +2319,25 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="23">
+      <c r="A4" s="24">
         <v>90</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="24">
         <v>2532</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="24">
         <v>483.4</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="24">
         <v>6</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="24">
         <v>9.6</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="24">
         <v>34</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="24">
         <v>37.59</v>
       </c>
       <c r="H4" s="25">
@@ -2362,12 +2362,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="31.4214285714286" customWidth="true"/>
+    <col min="2" max="2" width="31.425" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.5" spans="1:12">
+    <row r="1" ht="18.75" spans="1:12">
       <c r="A1" s="12" t="s">
         <v>41</v>
       </c>
@@ -2383,7 +2383,7 @@
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" ht="16" spans="1:12">
+    <row r="2" ht="14.25" spans="1:12">
       <c r="A2" s="13" t="s">
         <v>42</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" ht="34" spans="1:12">
+    <row r="3" ht="28.5" spans="1:12">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="15" t="s">
@@ -2455,7 +2455,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" ht="16" spans="1:12">
+    <row r="4" ht="14.25" spans="1:12">
       <c r="A4" s="13">
         <v>1</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="5" ht="16" spans="1:12">
+    <row r="5" ht="14.25" spans="1:12">
       <c r="A5" s="16" t="s">
         <v>49</v>
       </c>
@@ -2509,7 +2509,7 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
     </row>
-    <row r="6" ht="16" spans="1:12">
+    <row r="6" ht="14.25" spans="1:12">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -2523,7 +2523,7 @@
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" ht="16" spans="1:12">
+    <row r="7" ht="14.25" spans="1:12">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -2537,7 +2537,7 @@
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
     </row>
-    <row r="8" ht="18.5" spans="1:12">
+    <row r="8" ht="18.75" spans="1:12">
       <c r="A8" s="12" t="s">
         <v>50</v>
       </c>
@@ -2553,7 +2553,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" ht="16" spans="1:12">
+    <row r="9" ht="14.25" spans="1:12">
       <c r="A9" s="13" t="s">
         <v>42</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" ht="34" spans="1:12">
+    <row r="10" ht="28.5" spans="1:12">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="15" t="s">
@@ -2625,7 +2625,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" ht="16" spans="1:12">
+    <row r="11" ht="14.25" spans="1:12">
       <c r="A11" s="13">
         <v>1</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="12" ht="16" spans="1:12">
+    <row r="12" ht="14.25" spans="1:12">
       <c r="A12" s="16" t="s">
         <v>54</v>
       </c>
@@ -2704,9 +2704,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" ht="34" customHeight="true" spans="1:5">
+    <row r="1" ht="34" customHeight="1" spans="1:5">
       <c r="A1" s="9" t="s">
         <v>55</v>
       </c>
@@ -2791,9 +2791,9 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" ht="16" spans="1:13">
+    <row r="1" ht="14.25" spans="1:13">
       <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
@@ -2810,7 +2810,7 @@
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
-    <row r="2" ht="16" spans="1:13">
+    <row r="2" ht="14.25" spans="1:13">
       <c r="A2" s="8" t="s">
         <v>62</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" ht="16" spans="1:13">
+    <row r="3" ht="14.25" spans="1:13">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -2866,7 +2866,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" ht="16" spans="1:13">
+    <row r="4" ht="14.25" spans="1:13">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
         <v>75</v>
@@ -2905,7 +2905,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" ht="16" spans="1:13">
+    <row r="5" ht="14.25" spans="1:13">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2920,7 +2920,7 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" ht="16" spans="1:13">
+    <row r="6" ht="14.25" spans="1:13">
       <c r="A6" s="7" t="s">
         <v>87</v>
       </c>
@@ -2937,7 +2937,7 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" ht="16" spans="1:13">
+    <row r="7" ht="14.25" spans="1:13">
       <c r="A7" s="8" t="s">
         <v>62</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" ht="16" spans="1:13">
+    <row r="8" ht="14.25" spans="1:13">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -2975,7 +2975,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" ht="16" spans="1:13">
+    <row r="9" ht="14.25" spans="1:13">
       <c r="A9" s="7" t="s">
         <v>91</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" ht="16" spans="1:13">
+    <row r="10" ht="14.25" spans="1:13">
       <c r="A10" s="8" t="s">
         <v>62</v>
       </c>
@@ -3015,7 +3015,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" ht="16" spans="1:13">
+    <row r="11" ht="14.25" spans="1:13">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -3030,7 +3030,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" ht="16" spans="1:13">
+    <row r="12" ht="14.25" spans="1:13">
       <c r="A12" s="7" t="s">
         <v>95</v>
       </c>
@@ -3047,7 +3047,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" ht="16" spans="1:13">
+    <row r="13" ht="14.25" spans="1:13">
       <c r="A13" s="8" t="s">
         <v>96</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" ht="16" spans="1:13">
+    <row r="14" ht="14.25" spans="1:13">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -3085,7 +3085,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" ht="16" spans="1:13">
+    <row r="15" ht="14.25" spans="1:13">
       <c r="A15" s="8" t="s">
         <v>100</v>
       </c>
@@ -3110,7 +3110,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" ht="16" spans="1:13">
+    <row r="16" ht="14.25" spans="1:13">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -3140,38 +3140,37 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5"/>
   <cols>
-    <col min="4" max="4" width="10.8571428571429" customWidth="true"/>
-    <col min="5" max="5" width="13" customWidth="true"/>
-    <col min="6" max="6" width="12.5714285714286" customWidth="true"/>
-    <col min="7" max="7" width="9" customWidth="true"/>
-    <col min="8" max="8" width="10.3571428571429" customWidth="true"/>
-    <col min="9" max="9" width="10.1428571428571" customWidth="true"/>
-    <col min="10" max="10" width="11.3571428571429" customWidth="true"/>
-    <col min="11" max="11" width="13.6428571428571" customWidth="true"/>
-    <col min="12" max="12" width="14.2857142857143" customWidth="true"/>
-    <col min="13" max="13" width="11.5714285714286" customWidth="true"/>
-    <col min="16" max="16" width="12.3571428571429" customWidth="true"/>
+    <col min="4" max="4" width="10.8583333333333" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="12.575" customWidth="1"/>
+    <col min="7" max="8" width="13.6416666666667" customWidth="1"/>
+    <col min="9" max="9" width="10.1416666666667" customWidth="1"/>
+    <col min="10" max="10" width="11.3583333333333" customWidth="1"/>
+    <col min="11" max="11" width="13.6416666666667" customWidth="1"/>
+    <col min="12" max="12" width="14.2833333333333" customWidth="1"/>
+    <col min="13" max="13" width="11.575" customWidth="1"/>
+    <col min="16" max="16" width="12.3583333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.5" spans="1:20">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="16.5" spans="1:16">
+      <c r="A1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -3210,38 +3209,18 @@
       <c r="P1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" ht="14.5" spans="1:20">
-      <c r="A2" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="5">
         <v>2814</v>
       </c>
-      <c r="F2" s="5">
+      <c r="B2" s="5">
         <v>28</v>
       </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -3252,30 +3231,18 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-    </row>
-    <row r="3" ht="14.5" spans="1:20">
-      <c r="A3" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5">
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="5">
         <v>2532.6</v>
       </c>
-      <c r="F3" s="5">
+      <c r="B3" s="5">
         <v>27</v>
       </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -3286,30 +3253,18 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-    </row>
-    <row r="4" ht="14.5" spans="1:20">
-      <c r="A4" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5">
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="5">
         <v>2251.2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="B4" s="5">
         <v>26</v>
       </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -3320,30 +3275,18 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-    </row>
-    <row r="5" ht="14.5" spans="1:20">
-      <c r="A5" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3</v>
-      </c>
-      <c r="E5" s="5">
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="5">
         <v>1969.8</v>
       </c>
-      <c r="F5" s="5">
+      <c r="B5" s="5">
         <v>25</v>
       </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -3354,30 +3297,18 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-    </row>
-    <row r="6" ht="14.5" spans="1:20">
-      <c r="A6" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5">
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="5">
         <v>1688.4</v>
       </c>
-      <c r="F6" s="5">
+      <c r="B6" s="5">
         <v>24</v>
       </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -3388,30 +3319,18 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-    </row>
-    <row r="7" ht="14.5" spans="1:20">
-      <c r="A7" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>5</v>
-      </c>
-      <c r="E7" s="5">
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="5">
         <v>1407</v>
       </c>
-      <c r="F7" s="5">
+      <c r="B7" s="5">
         <v>23</v>
       </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -3422,30 +3341,18 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-    </row>
-    <row r="8" ht="14.5" spans="1:20">
-      <c r="A8" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>6</v>
-      </c>
-      <c r="E8" s="5">
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="5">
         <v>1125.6</v>
       </c>
-      <c r="F8" s="5">
+      <c r="B8" s="5">
         <v>22</v>
       </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -3456,30 +3363,18 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-    </row>
-    <row r="9" ht="14.5" spans="1:20">
-      <c r="A9" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5">
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="5">
         <v>844.2</v>
       </c>
-      <c r="F9" s="5">
+      <c r="B9" s="5">
         <v>20</v>
       </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -3490,30 +3385,18 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-    </row>
-    <row r="10" ht="14.5" spans="1:20">
-      <c r="A10" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>8</v>
-      </c>
-      <c r="E10" s="5">
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="5">
         <v>562.8</v>
       </c>
-      <c r="F10" s="5">
+      <c r="B10" s="5">
         <v>18</v>
       </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -3524,30 +3407,18 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-    </row>
-    <row r="11" ht="14.5" spans="1:20">
-      <c r="A11" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
-        <v>9</v>
-      </c>
-      <c r="E11" s="6">
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="6">
         <v>281.4</v>
       </c>
-      <c r="F11" s="6">
+      <c r="B11" s="6">
         <v>16</v>
       </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -3558,10 +3429,6 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3578,219 +3445,219 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="7" max="7" width="16.25" customWidth="true"/>
+    <col min="7" max="7" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16" spans="1:7">
+    <row r="1" ht="17.25" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" ht="16" spans="1:7">
+    <row r="2" ht="14.25" spans="1:7">
       <c r="A2" s="1">
         <v>2021</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>0</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>2814</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>28</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" ht="16" spans="1:7">
+    <row r="3" ht="14.25" spans="1:7">
       <c r="A3" s="1">
         <v>2021</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>2532.6</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>27</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" ht="16" spans="1:7">
+    <row r="4" ht="14.25" spans="1:7">
       <c r="A4" s="1">
         <v>2021</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>2251.2</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>26</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" ht="16" spans="1:7">
+    <row r="5" ht="14.25" spans="1:7">
       <c r="A5" s="1">
         <v>2021</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>1969.8</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>25</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" ht="16" spans="1:7">
+    <row r="6" ht="14.25" spans="1:7">
       <c r="A6" s="1">
         <v>2021</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>4</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>1688.4</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>24</v>
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" ht="16" spans="1:7">
+    <row r="7" ht="14.25" spans="1:7">
       <c r="A7" s="1">
         <v>2021</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>5</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>1407</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>23</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" ht="16" spans="1:7">
+    <row r="8" ht="14.25" spans="1:7">
       <c r="A8" s="1">
         <v>2021</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>6</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>1125.6</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>22</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" ht="16" spans="1:7">
+    <row r="9" ht="14.25" spans="1:7">
       <c r="A9" s="1">
         <v>2021</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>1</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>7</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>844.2</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>20</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" ht="16" spans="1:7">
+    <row r="10" ht="14.25" spans="1:7">
       <c r="A10" s="1">
         <v>2021</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <v>8</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>562.8</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>18</v>
       </c>
       <c r="G10" s="1"/>

</xml_diff>